<commit_message>
Personal Finance Tracker Dashboard
</commit_message>
<xml_diff>
--- a/Excel/Finance_Tracker_Dashboard.xlsx
+++ b/Excel/Finance_Tracker_Dashboard.xlsx
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="178" r:id="rId6"/>
-    <pivotCache cacheId="190" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1797" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="156">
   <si>
     <t>Month</t>
   </si>
@@ -826,15 +826,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -849,6 +840,15 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1453,7 +1453,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Sheet4 (2)!PivotTable3</c:name>
+    <c:name>[Finance_Tracker_Dashboard.xlsx]Sheet4 (2)!PivotTable3</c:name>
     <c:fmtId val="3"/>
   </c:pivotSource>
   <c:chart>
@@ -1694,6 +1694,291 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="56"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="57"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="58"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="59"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="60"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="61"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="62"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="63"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="64"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="65"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="66"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="67"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="68"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="69"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="70"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="71"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="72"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="73"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="74"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="75"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="76"/>
@@ -2385,291 +2670,6 @@
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="122"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="123"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="124"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="125"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="126"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="127"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="128"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="129"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="130"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="131"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="132"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="133"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="134"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="135"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="136"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="137"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="138"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="139"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="140"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -4055,7 +4055,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Sheet4 (3)!PivotTable6</c:name>
+    <c:name>[Finance_Tracker_Dashboard.xlsx]Sheet4 (3)!PivotTable6</c:name>
     <c:fmtId val="5"/>
   </c:pivotSource>
   <c:chart>
@@ -4202,7 +4202,7 @@
         <c:idx val="24"/>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="33"/>
+        <c:idx val="25"/>
         <c:spPr>
           <a:gradFill rotWithShape="1">
             <a:gsLst>
@@ -4235,6 +4235,134 @@
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent6">
+                  <a:tint val="64000"/>
+                  <a:lumMod val="118000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent6">
+                  <a:tint val="92000"/>
+                  <a:alpha val="100000"/>
+                  <a:lumMod val="110000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:shade val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent6">
+                  <a:tint val="64000"/>
+                  <a:lumMod val="118000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent6">
+                  <a:tint val="92000"/>
+                  <a:alpha val="100000"/>
+                  <a:lumMod val="110000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:shade val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent6">
+                  <a:tint val="64000"/>
+                  <a:lumMod val="118000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent6">
+                  <a:tint val="92000"/>
+                  <a:alpha val="100000"/>
+                  <a:lumMod val="110000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:shade val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="29"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent6">
+                  <a:tint val="64000"/>
+                  <a:lumMod val="118000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent6">
+                  <a:tint val="92000"/>
+                  <a:alpha val="100000"/>
+                  <a:lumMod val="110000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:shade val="95000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -4287,6 +4415,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5274-4F5F-9CCE-B86968A23D25}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4320,6 +4453,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5274-4F5F-9CCE-B86968A23D25}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4353,6 +4491,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5274-4F5F-9CCE-B86968A23D25}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -4389,46 +4532,35 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5274-4F5F-9CCE-B86968A23D25}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Sheet4 (3)'!$B$4:$B$12</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>'Sheet4 (3)'!$B$4:$B$8</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>E-commerce</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Google Adsecne</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>My Shop</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Salary</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>E-commerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Google Adsecne</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>My Shop</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Salary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet4 (3)'!$C$4:$C$12</c:f>
+              <c:f>'Sheet4 (3)'!$C$4:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -4572,7 +4704,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Sheet2!PivotTable1</c:name>
+    <c:name>[Finance_Tracker_Dashboard.xlsx]Sheet2!PivotTable1</c:name>
     <c:fmtId val="9"/>
   </c:pivotSource>
   <c:chart>
@@ -4695,6 +4827,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
           <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -4723,6 +4858,9 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
           <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent3"/>
@@ -4737,6 +4875,66 @@
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:shade val="76000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:miter lim="800000"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:tint val="77000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
@@ -5275,7 +5473,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Sheet2!PivotTable1</c:name>
+    <c:name>[Finance_Tracker_Dashboard.xlsx]Sheet2!PivotTable1</c:name>
     <c:fmtId val="7"/>
   </c:pivotSource>
   <c:chart>
@@ -5290,6 +5488,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -5316,6 +5517,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -5772,7 +5976,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5869,7 +6072,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Sheet4 (2)!PivotTable6</c:name>
+    <c:name>[Finance_Tracker_Dashboard.xlsx]Sheet4 (2)!PivotTable6</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -6756,7 +6959,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6853,7 +7055,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Sheet4 (2)!PivotTable3</c:name>
+    <c:name>[Finance_Tracker_Dashboard.xlsx]Sheet4 (2)!PivotTable3</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -8500,7 +8702,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8597,12 +8798,11 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Dashboard.xlsx]Sheet4 (3)!PivotTable6</c:name>
+    <c:name>[Finance_Tracker_Dashboard.xlsx]Sheet4 (3)!PivotTable6</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8936,44 +9136,28 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Sheet4 (3)'!$B$4:$B$12</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>'Sheet4 (3)'!$B$4:$B$8</c:f>
+              <c:strCache>
                 <c:ptCount val="4"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Income</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>E-commerce</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Google Adsecne</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>My Shop</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Salary</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>E-commerce</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Google Adsecne</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>My Shop</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Salary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sheet4 (3)'!$C$4:$C$12</c:f>
+              <c:f>'Sheet4 (3)'!$C$4:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -9128,7 +9312,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13212,8 +13395,8 @@
       <xdr:row>24</xdr:row>
       <xdr:rowOff>126999</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="7" name="Month"/>
@@ -13230,7 +13413,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -19645,7 +19828,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="190" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="A1:C15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0" nonAutoSortDefault="1">
@@ -19748,7 +19931,7 @@
   <dataFields count="1">
     <dataField name="Sum of Amount" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
+  <chartFormats count="8">
     <chartFormat chart="8" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -19821,6 +20004,30 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="9" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -19832,7 +20039,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="178" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="AA1:AF16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0" sortType="ascending" defaultSubtotal="0"/>
@@ -20084,7 +20291,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="178" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A1:U6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -20522,7 +20729,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="118" series="1">
+    <chartFormat chart="3" format="99" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20534,7 +20741,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="119" series="1">
+    <chartFormat chart="3" format="100" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20546,7 +20753,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="120" series="1">
+    <chartFormat chart="3" format="101" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20558,7 +20765,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="121" series="1">
+    <chartFormat chart="3" format="102" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20570,7 +20777,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="122" series="1">
+    <chartFormat chart="3" format="103" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20582,7 +20789,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="123" series="1">
+    <chartFormat chart="3" format="104" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20594,7 +20801,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="124" series="1">
+    <chartFormat chart="3" format="105" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20606,7 +20813,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="125" series="1">
+    <chartFormat chart="3" format="106" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20618,7 +20825,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="126" series="1">
+    <chartFormat chart="3" format="107" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20630,7 +20837,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="127" series="1">
+    <chartFormat chart="3" format="108" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20642,7 +20849,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="128" series="1">
+    <chartFormat chart="3" format="109" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20654,7 +20861,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="129" series="1">
+    <chartFormat chart="3" format="110" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20666,7 +20873,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="130" series="1">
+    <chartFormat chart="3" format="111" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20678,7 +20885,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="131" series="1">
+    <chartFormat chart="3" format="112" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20690,7 +20897,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="132" series="1">
+    <chartFormat chart="3" format="113" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20702,7 +20909,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="133" series="1">
+    <chartFormat chart="3" format="114" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20714,7 +20921,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="134" series="1">
+    <chartFormat chart="3" format="115" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20726,7 +20933,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="135" series="1">
+    <chartFormat chart="3" format="116" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20738,7 +20945,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="136" series="1">
+    <chartFormat chart="3" format="117" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20750,7 +20957,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="137" series="1">
+    <chartFormat chart="3" format="118" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20762,7 +20969,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="138" series="1">
+    <chartFormat chart="3" format="119" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20774,7 +20981,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="139" series="1">
+    <chartFormat chart="3" format="120" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20786,7 +20993,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="3" format="140" series="1">
+    <chartFormat chart="3" format="121" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -20809,8 +21016,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="178" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="B3:C12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="B3:C8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0" sortType="ascending" defaultSubtotal="0"/>
     <pivotField showAll="0" nonAutoSortDefault="1">
@@ -20842,7 +21049,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="3">
         <item h="1" x="0"/>
         <item x="1"/>
@@ -20852,29 +21059,29 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
       <items count="24">
-        <item x="0"/>
+        <item h="1" x="0"/>
         <item x="21"/>
-        <item x="1"/>
-        <item x="12"/>
+        <item h="1" x="1"/>
+        <item h="1" x="12"/>
         <item x="22"/>
-        <item x="16"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="14"/>
+        <item h="1" x="16"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item h="1" x="14"/>
         <item x="20"/>
-        <item x="8"/>
-        <item x="11"/>
-        <item x="15"/>
-        <item x="5"/>
-        <item x="17"/>
-        <item x="6"/>
+        <item h="1" x="8"/>
+        <item h="1" x="11"/>
+        <item h="1" x="15"/>
+        <item h="1" x="5"/>
+        <item h="1" x="17"/>
+        <item h="1" x="6"/>
         <item x="19"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="18"/>
-        <item x="7"/>
-        <item x="13"/>
-        <item x="4"/>
+        <item h="1" x="10"/>
+        <item h="1" x="9"/>
+        <item h="1" x="18"/>
+        <item h="1" x="7"/>
+        <item h="1" x="13"/>
+        <item h="1" x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -20882,34 +21089,21 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="1">
     <field x="4"/>
-    <field x="2"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="5">
     <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
       <x v="1"/>
     </i>
     <i>
       <x v="4"/>
     </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
     <i>
       <x v="9"/>
     </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
     <i>
       <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
     </i>
     <i t="grand">
       <x/>
@@ -20988,7 +21182,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="5" format="33" series="1">
+    <chartFormat chart="5" format="25" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -21417,11 +21611,11 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="F6" s="20">
+      <c r="F6" s="29">
         <f>GETPIVOTDATA("Amount",'Sheet4 (2)'!$A$1)</f>
         <v>1981</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="30">
         <f>GETPIVOTDATA("Amount",'Sheet4 (3)'!$B$3)</f>
         <v>2938</v>
       </c>
@@ -21429,18 +21623,18 @@
     </row>
     <row r="7" spans="2:18" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7"/>
-      <c r="C7" s="22">
+      <c r="C7" s="31">
         <f>GETPIVOTDATA("Amount",'Sheet4 (3)'!$B$3)-GETPIVOTDATA("Amount",'Sheet4 (2)'!$A$1)</f>
         <v>957</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="F7" s="20"/>
-      <c r="H7" s="21"/>
+      <c r="F7" s="29"/>
+      <c r="H7" s="30"/>
       <c r="R7"/>
     </row>
     <row r="8" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -21491,7 +21685,7 @@
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="R16" s="23" t="s">
+      <c r="R16" s="20" t="s">
         <v>142</v>
       </c>
     </row>
@@ -21504,13 +21698,13 @@
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="S18" s="26" t="s">
+      <c r="S18" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="U18" s="27" t="s">
+      <c r="U18" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="W18" s="30" t="s">
+      <c r="W18" s="27" t="s">
         <v>32</v>
       </c>
     </row>
@@ -21518,15 +21712,15 @@
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="S19" s="28">
+      <c r="S19" s="25">
         <f>GETPIVOTDATA("Amount",'Sheet4 (2)'!$A$1,"Category","Housing")</f>
         <v>865</v>
       </c>
-      <c r="U19" s="29">
+      <c r="U19" s="26">
         <f>GETPIVOTDATA("Amount",'Sheet4 (2)'!$A$1,"Category","Personal")</f>
         <v>492</v>
       </c>
-      <c r="W19" s="31">
+      <c r="W19" s="28">
         <f>GETPIVOTDATA("Amount",'Sheet4 (2)'!$A$1,"Category","Transportation")</f>
         <v>624</v>
       </c>
@@ -21535,17 +21729,17 @@
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="S20" s="24"/>
+      <c r="S20" s="21"/>
       <c r="U20" s="8"/>
-      <c r="W20" s="25"/>
+      <c r="W20" s="22"/>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="S21" s="24"/>
+      <c r="S21" s="21"/>
       <c r="U21" s="8"/>
-      <c r="W21" s="25"/>
+      <c r="W21" s="22"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
@@ -22453,7 +22647,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C12"/>
+  <dimension ref="B3:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -22462,7 +22656,7 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8"/>
-    <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
     <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="7.125" customWidth="1"/>
@@ -22514,66 +22708,34 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>40</v>
+      <c r="B5" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C5" s="6">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="6">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
-        <v>40</v>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C7" s="6">
-        <v>140</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
-        <v>43</v>
+        <v>137</v>
       </c>
       <c r="C8" s="6">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="6">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="6">
-        <v>2510</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="6">
-        <v>2510</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="6">
         <v>2938</v>
       </c>
     </row>
@@ -22591,7 +22753,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="9.25" customWidth="1"/>
@@ -22602,7 +22764,7 @@
     <col min="7" max="7" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>140</v>
       </c>
@@ -22628,7 +22790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -22654,7 +22816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -22680,7 +22842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -22706,7 +22868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -22732,7 +22894,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -22758,7 +22920,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -22784,7 +22946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -22810,7 +22972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -22836,7 +22998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -22862,7 +23024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -22888,7 +23050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -22914,7 +23076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -22940,7 +23102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -22966,7 +23128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -22992,7 +23154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -23018,7 +23180,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -23044,7 +23206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -23070,7 +23232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -23096,7 +23258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -23122,7 +23284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -23148,7 +23310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -23174,7 +23336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -23194,7 +23356,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -23214,7 +23376,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -23234,7 +23396,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -23254,7 +23416,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -23280,7 +23442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -23306,7 +23468,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -23332,7 +23494,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -23358,7 +23520,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2</v>
       </c>
@@ -23384,7 +23546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -23410,7 +23572,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -23436,7 +23598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -23462,7 +23624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -23488,7 +23650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -23514,7 +23676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -23540,7 +23702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -23566,7 +23728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -23592,7 +23754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -23618,7 +23780,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -23644,7 +23806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
@@ -23670,7 +23832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -23696,7 +23858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -23722,7 +23884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -23748,7 +23910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -23774,7 +23936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -23800,7 +23962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -23820,7 +23982,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -23840,7 +24002,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -23860,7 +24022,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -23880,7 +24042,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -23906,7 +24068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>3</v>
       </c>
@@ -23932,7 +24094,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>3</v>
       </c>
@@ -23958,7 +24120,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>3</v>
       </c>
@@ -23984,7 +24146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -24010,7 +24172,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -24036,7 +24198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>3</v>
       </c>
@@ -24062,7 +24224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
@@ -24088,7 +24250,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3</v>
       </c>
@@ -24114,7 +24276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
@@ -24140,7 +24302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3</v>
       </c>
@@ -24166,7 +24328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3</v>
       </c>
@@ -24192,7 +24354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3</v>
       </c>
@@ -24218,7 +24380,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
@@ -24244,7 +24406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3</v>
       </c>
@@ -24270,7 +24432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3</v>
       </c>
@@ -24296,7 +24458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -24322,7 +24484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3</v>
       </c>
@@ -24348,7 +24510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3</v>
       </c>
@@ -24374,7 +24536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3</v>
       </c>
@@ -24400,7 +24562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3</v>
       </c>
@@ -24426,7 +24588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3</v>
       </c>
@@ -24446,7 +24608,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3</v>
       </c>
@@ -24466,7 +24628,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>3</v>
       </c>
@@ -24486,7 +24648,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3</v>
       </c>
@@ -24506,7 +24668,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4</v>
       </c>
@@ -24532,7 +24694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4</v>
       </c>
@@ -24558,7 +24720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4</v>
       </c>
@@ -24584,7 +24746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4</v>
       </c>
@@ -24610,7 +24772,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -24636,7 +24798,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4</v>
       </c>
@@ -24662,7 +24824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -24688,7 +24850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
@@ -24714,7 +24876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4</v>
       </c>
@@ -24740,7 +24902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4</v>
       </c>
@@ -24766,7 +24928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -24792,7 +24954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -24818,7 +24980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
@@ -24844,7 +25006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>4</v>
       </c>
@@ -24870,7 +25032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -24896,7 +25058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
@@ -24922,7 +25084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
@@ -24948,7 +25110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
@@ -24974,7 +25136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4</v>
       </c>
@@ -25000,7 +25162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4</v>
       </c>
@@ -25026,7 +25188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4</v>
       </c>
@@ -25052,7 +25214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>4</v>
       </c>
@@ -25072,7 +25234,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4</v>
       </c>
@@ -25092,7 +25254,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>4</v>
       </c>
@@ -25112,7 +25274,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>4</v>
       </c>
@@ -25132,7 +25294,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>5</v>
       </c>
@@ -25158,7 +25320,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>5</v>
       </c>
@@ -25184,7 +25346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>5</v>
       </c>
@@ -25210,7 +25372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>5</v>
       </c>
@@ -25236,7 +25398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>5</v>
       </c>
@@ -25262,7 +25424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>5</v>
       </c>
@@ -25288,7 +25450,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>5</v>
       </c>
@@ -25314,7 +25476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>5</v>
       </c>
@@ -25340,7 +25502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>5</v>
       </c>
@@ -25366,7 +25528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>5</v>
       </c>
@@ -25392,7 +25554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>5</v>
       </c>
@@ -25418,7 +25580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>5</v>
       </c>
@@ -25444,7 +25606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>5</v>
       </c>
@@ -25470,7 +25632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>5</v>
       </c>
@@ -25496,7 +25658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>5</v>
       </c>
@@ -25522,7 +25684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>5</v>
       </c>
@@ -25548,7 +25710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>5</v>
       </c>
@@ -25574,7 +25736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>5</v>
       </c>
@@ -25600,7 +25762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>5</v>
       </c>
@@ -25626,7 +25788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>5</v>
       </c>
@@ -25652,7 +25814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>5</v>
       </c>
@@ -25678,7 +25840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>5</v>
       </c>
@@ -25698,7 +25860,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>5</v>
       </c>
@@ -25718,7 +25880,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>5</v>
       </c>
@@ -25738,7 +25900,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>5</v>
       </c>
@@ -25758,7 +25920,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>6</v>
       </c>
@@ -25784,7 +25946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>6</v>
       </c>
@@ -25810,7 +25972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>6</v>
       </c>
@@ -25836,7 +25998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>6</v>
       </c>
@@ -25862,7 +26024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>6</v>
       </c>
@@ -25888,7 +26050,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>6</v>
       </c>
@@ -25914,7 +26076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>6</v>
       </c>
@@ -25940,7 +26102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>6</v>
       </c>
@@ -25966,7 +26128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>6</v>
       </c>
@@ -25992,7 +26154,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>6</v>
       </c>
@@ -26018,7 +26180,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>6</v>
       </c>
@@ -26044,7 +26206,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>6</v>
       </c>
@@ -26070,7 +26232,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>6</v>
       </c>
@@ -26096,7 +26258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>6</v>
       </c>
@@ -26122,7 +26284,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>6</v>
       </c>
@@ -26148,7 +26310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>6</v>
       </c>
@@ -26174,7 +26336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>6</v>
       </c>
@@ -26200,7 +26362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>6</v>
       </c>
@@ -26226,7 +26388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>6</v>
       </c>
@@ -26252,7 +26414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>6</v>
       </c>
@@ -26278,7 +26440,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>6</v>
       </c>
@@ -26304,7 +26466,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>6</v>
       </c>
@@ -26324,7 +26486,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>6</v>
       </c>
@@ -26344,7 +26506,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>6</v>
       </c>
@@ -26364,7 +26526,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>6</v>
       </c>
@@ -26384,7 +26546,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>7</v>
       </c>
@@ -26410,7 +26572,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>7</v>
       </c>
@@ -26436,7 +26598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>7</v>
       </c>
@@ -26462,7 +26624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>7</v>
       </c>
@@ -26488,7 +26650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>7</v>
       </c>
@@ -26514,7 +26676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>7</v>
       </c>
@@ -26540,7 +26702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>7</v>
       </c>
@@ -26566,7 +26728,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>7</v>
       </c>
@@ -26592,7 +26754,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>7</v>
       </c>
@@ -26618,7 +26780,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>7</v>
       </c>
@@ -26644,7 +26806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>7</v>
       </c>
@@ -26670,7 +26832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>7</v>
       </c>
@@ -26696,7 +26858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>7</v>
       </c>
@@ -26722,7 +26884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>7</v>
       </c>
@@ -26748,7 +26910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>7</v>
       </c>
@@ -26774,7 +26936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>7</v>
       </c>
@@ -26800,7 +26962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>7</v>
       </c>
@@ -26826,7 +26988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>7</v>
       </c>
@@ -26852,7 +27014,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>7</v>
       </c>
@@ -26878,7 +27040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>7</v>
       </c>
@@ -26904,7 +27066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>7</v>
       </c>
@@ -26930,7 +27092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>7</v>
       </c>
@@ -26950,7 +27112,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>7</v>
       </c>
@@ -26970,7 +27132,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>7</v>
       </c>
@@ -26990,7 +27152,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>7</v>
       </c>
@@ -27010,7 +27172,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>8</v>
       </c>
@@ -27036,7 +27198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>8</v>
       </c>
@@ -27062,7 +27224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>8</v>
       </c>
@@ -27088,7 +27250,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>8</v>
       </c>
@@ -27114,7 +27276,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>8</v>
       </c>
@@ -27140,7 +27302,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>8</v>
       </c>
@@ -27166,7 +27328,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>8</v>
       </c>
@@ -27192,7 +27354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>8</v>
       </c>
@@ -27218,7 +27380,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>8</v>
       </c>
@@ -27244,7 +27406,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>8</v>
       </c>
@@ -27270,7 +27432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>8</v>
       </c>
@@ -27296,7 +27458,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>8</v>
       </c>
@@ -27322,7 +27484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>8</v>
       </c>
@@ -27348,7 +27510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>8</v>
       </c>
@@ -27374,7 +27536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>8</v>
       </c>
@@ -27400,7 +27562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>8</v>
       </c>
@@ -27426,7 +27588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>8</v>
       </c>
@@ -27452,7 +27614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>8</v>
       </c>
@@ -27478,7 +27640,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>8</v>
       </c>
@@ -27504,7 +27666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>8</v>
       </c>
@@ -27530,7 +27692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>8</v>
       </c>
@@ -27556,7 +27718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>8</v>
       </c>
@@ -27576,7 +27738,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>8</v>
       </c>
@@ -27596,7 +27758,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>8</v>
       </c>
@@ -27616,7 +27778,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>8</v>
       </c>
@@ -27636,7 +27798,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>9</v>
       </c>
@@ -27662,7 +27824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>9</v>
       </c>
@@ -27688,7 +27850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>9</v>
       </c>
@@ -27714,7 +27876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>9</v>
       </c>
@@ -27740,7 +27902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>9</v>
       </c>
@@ -27766,7 +27928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>9</v>
       </c>
@@ -27792,7 +27954,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>9</v>
       </c>
@@ -27818,7 +27980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="209" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>9</v>
       </c>
@@ -27844,7 +28006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="210" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>9</v>
       </c>
@@ -27870,7 +28032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="211" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>9</v>
       </c>
@@ -27896,7 +28058,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="212" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>9</v>
       </c>
@@ -27922,7 +28084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>9</v>
       </c>
@@ -27948,7 +28110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="214" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>9</v>
       </c>
@@ -27974,7 +28136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="215" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>9</v>
       </c>
@@ -28000,7 +28162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="216" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>9</v>
       </c>
@@ -28026,7 +28188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="217" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>9</v>
       </c>
@@ -28052,7 +28214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="218" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>9</v>
       </c>
@@ -28078,7 +28240,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="219" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>9</v>
       </c>
@@ -28104,7 +28266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>9</v>
       </c>
@@ -28130,7 +28292,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>9</v>
       </c>
@@ -28156,7 +28318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>9</v>
       </c>
@@ -28182,7 +28344,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>9</v>
       </c>
@@ -28202,7 +28364,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>9</v>
       </c>
@@ -28222,7 +28384,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>9</v>
       </c>
@@ -28242,7 +28404,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>9</v>
       </c>
@@ -28262,7 +28424,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>10</v>
       </c>
@@ -28288,7 +28450,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>10</v>
       </c>
@@ -28314,7 +28476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>10</v>
       </c>
@@ -28340,7 +28502,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>10</v>
       </c>
@@ -28366,7 +28528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>10</v>
       </c>
@@ -28392,7 +28554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>10</v>
       </c>
@@ -28418,7 +28580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>10</v>
       </c>
@@ -28444,7 +28606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>10</v>
       </c>
@@ -28470,7 +28632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>10</v>
       </c>
@@ -28496,7 +28658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>10</v>
       </c>
@@ -28522,7 +28684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>10</v>
       </c>
@@ -28548,7 +28710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>10</v>
       </c>
@@ -28574,7 +28736,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>10</v>
       </c>
@@ -28600,7 +28762,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>10</v>
       </c>
@@ -28626,7 +28788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="241" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>10</v>
       </c>
@@ -28652,7 +28814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="242" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>10</v>
       </c>
@@ -28678,7 +28840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="243" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>10</v>
       </c>
@@ -28704,7 +28866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="244" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>10</v>
       </c>
@@ -28730,7 +28892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="245" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>10</v>
       </c>
@@ -28756,7 +28918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="246" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>10</v>
       </c>
@@ -28782,7 +28944,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>10</v>
       </c>
@@ -28808,7 +28970,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="248" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>10</v>
       </c>
@@ -28828,7 +28990,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="249" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>10</v>
       </c>
@@ -28848,7 +29010,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="250" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>10</v>
       </c>
@@ -28868,7 +29030,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="251" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>10</v>
       </c>
@@ -28888,7 +29050,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="252" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>11</v>
       </c>
@@ -28914,7 +29076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>11</v>
       </c>
@@ -28943,7 +29105,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="254" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>11</v>
       </c>
@@ -28969,7 +29131,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>11</v>
       </c>
@@ -28995,7 +29157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>11</v>
       </c>
@@ -29021,7 +29183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>11</v>
       </c>
@@ -29047,7 +29209,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="258" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>11</v>
       </c>
@@ -29073,7 +29235,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>11</v>
       </c>
@@ -29099,7 +29261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>11</v>
       </c>
@@ -29125,7 +29287,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>11</v>
       </c>
@@ -29151,7 +29313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="262" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>11</v>
       </c>
@@ -29177,7 +29339,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>11</v>
       </c>
@@ -29203,7 +29365,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="264" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>11</v>
       </c>
@@ -29229,7 +29391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>11</v>
       </c>
@@ -29255,7 +29417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="266" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>11</v>
       </c>
@@ -29281,7 +29443,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>11</v>
       </c>
@@ -29307,7 +29469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>11</v>
       </c>
@@ -29333,7 +29495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>11</v>
       </c>
@@ -29359,7 +29521,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>11</v>
       </c>
@@ -29385,7 +29547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="271" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>11</v>
       </c>
@@ -29411,7 +29573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>11</v>
       </c>
@@ -29437,7 +29599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>11</v>
       </c>
@@ -29457,7 +29619,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>11</v>
       </c>
@@ -29477,7 +29639,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="275" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>11</v>
       </c>
@@ -29497,7 +29659,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="276" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>11</v>
       </c>
@@ -29517,7 +29679,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="277" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>12</v>
       </c>
@@ -29543,7 +29705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="278" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>12</v>
       </c>
@@ -29569,7 +29731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>12</v>
       </c>
@@ -29595,7 +29757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="280" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>12</v>
       </c>
@@ -29621,7 +29783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="281" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>12</v>
       </c>
@@ -29647,7 +29809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="282" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>12</v>
       </c>
@@ -29673,7 +29835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="283" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>12</v>
       </c>
@@ -29699,7 +29861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="284" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>12</v>
       </c>
@@ -29725,7 +29887,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="285" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>12</v>
       </c>
@@ -29751,7 +29913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="286" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>12</v>
       </c>
@@ -29777,7 +29939,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="287" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>12</v>
       </c>
@@ -29803,7 +29965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="288" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>12</v>
       </c>
@@ -29829,7 +29991,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="289" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>12</v>
       </c>
@@ -29855,7 +30017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="290" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>12</v>
       </c>
@@ -29881,7 +30043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="291" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>12</v>
       </c>
@@ -29907,7 +30069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="292" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>12</v>
       </c>
@@ -29933,7 +30095,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>12</v>
       </c>
@@ -29959,7 +30121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="294" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>12</v>
       </c>
@@ -29985,7 +30147,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="295" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>12</v>
       </c>
@@ -30011,7 +30173,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="296" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>12</v>
       </c>
@@ -30037,7 +30199,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="297" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>12</v>
       </c>
@@ -30063,7 +30225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="298" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>12</v>
       </c>
@@ -30083,7 +30245,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="299" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>12</v>
       </c>
@@ -30103,7 +30265,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="300" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>12</v>
       </c>
@@ -30123,7 +30285,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="301" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>12</v>
       </c>

</xml_diff>